<commit_message>
fix user import script
</commit_message>
<xml_diff>
--- a/src/db/user.xlsx
+++ b/src/db/user.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t>姓名</t>
     <rPh sb="0" eb="1">
@@ -206,10 +206,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>HER</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>状态(1: 在职 2: 离职 3: 退休 0: 其他)</t>
     <rPh sb="0" eb="1">
       <t>zhuang tai</t>
@@ -253,6 +249,119 @@
     <rPh sb="0" eb="1">
       <t>xue li</t>
     </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>所在部门（必须填写系统中存在的部门）</t>
+    <rPh sb="0" eb="1">
+      <t>suo zai</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>bu men</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>bi xu</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>tian xie</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>xi tong</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>zhong</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>cun zai</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>de</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>bu men</t>
+    </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>角色（必须填写系统中存在的角色）</t>
+    <rPh sb="0" eb="1">
+      <t>jue se</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>bi xu</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>tian xie</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>xi tong</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>zhong</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>cun zai</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>de</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>jue se</t>
+    </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>HER</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>地服部分会</t>
+    <rPh sb="0" eb="1">
+      <t>di xia</t>
+    </rPh>
+    <rPh sb="1" eb="2">
+      <t>fu wu</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>bu men</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>fen</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>hui</t>
+    </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>普通会员</t>
+    <rPh sb="0" eb="1">
+      <t>pu tong</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>hui yuan</t>
+    </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>性别（1: 女 2: 男）</t>
+    <rPh sb="0" eb="1">
+      <t>xing bie</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>nü</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>nan</t>
+    </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2017-8-10</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2017-8-9</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -316,8 +425,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -595,26 +704,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.1640625" customWidth="1"/>
-    <col min="2" max="2" width="37" customWidth="1"/>
-    <col min="3" max="3" width="22.6640625" customWidth="1"/>
-    <col min="4" max="4" width="26.83203125" customWidth="1"/>
-    <col min="6" max="6" width="32.83203125" customWidth="1"/>
-    <col min="8" max="8" width="35.5" customWidth="1"/>
-    <col min="11" max="11" width="43.5" customWidth="1"/>
-    <col min="16" max="16" width="32.1640625" customWidth="1"/>
-    <col min="17" max="17" width="30.5" customWidth="1"/>
+    <col min="2" max="3" width="37" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" customWidth="1"/>
+    <col min="5" max="5" width="26.83203125" customWidth="1"/>
+    <col min="7" max="7" width="32.83203125" customWidth="1"/>
+    <col min="9" max="9" width="35.5" customWidth="1"/>
+    <col min="10" max="10" width="37.83203125" customWidth="1"/>
+    <col min="11" max="11" width="34" customWidth="1"/>
+    <col min="14" max="14" width="43.5" customWidth="1"/>
+    <col min="19" max="19" width="32.1640625" customWidth="1"/>
+    <col min="20" max="20" width="30.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -622,114 +733,132 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O1" t="s">
         <v>7</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>8</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>9</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>10</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="T1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" t="s">
+      <c r="U1" t="s">
         <v>11</v>
       </c>
-      <c r="S1" t="s">
+      <c r="V1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>16</v>
       </c>
       <c r="B2">
-        <v>18627894265</v>
-      </c>
-      <c r="C2" s="3">
-        <v>42957</v>
+        <v>15839888262</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
       </c>
       <c r="D2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
         <v>123</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>0</v>
       </c>
-      <c r="I2">
+      <c r="J2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2">
         <v>123</v>
       </c>
-      <c r="J2">
+      <c r="M2">
         <v>123</v>
       </c>
-      <c r="K2">
+      <c r="N2">
         <v>1</v>
       </c>
-      <c r="L2" t="s">
+      <c r="O2" t="s">
+        <v>19</v>
+      </c>
+      <c r="P2" t="s">
         <v>20</v>
       </c>
-      <c r="M2" t="s">
+      <c r="Q2" t="s">
         <v>21</v>
       </c>
-      <c r="N2" t="s">
+      <c r="R2" t="s">
         <v>22</v>
       </c>
-      <c r="O2" t="s">
+      <c r="S2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="U2">
+        <v>20</v>
+      </c>
+      <c r="V2" t="s">
         <v>23</v>
-      </c>
-      <c r="P2" s="3">
-        <v>42956</v>
-      </c>
-      <c r="Q2" s="3">
-        <v>42956</v>
-      </c>
-      <c r="R2">
-        <v>20</v>
-      </c>
-      <c r="S2" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>